<commit_message>
add period mode in update_akshare_file in SymbolData class
</commit_message>
<xml_diff>
--- a/steel/data/mid-stream/螺纹钢/螺纹钢期货价格.xlsx
+++ b/steel/data/mid-stream/螺纹钢/螺纹钢期货价格.xlsx
@@ -30,7 +30,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t>yVjpCgZpNvOHlEoAN60+iXcNR8qcjD2afR3U+XlDrUTEX5W5KWYQZl2WlS6znR8JdtRv8fy9hcGzGgX1t8jwbDwAx0EUQZsw3ZWNu8RJYhGO4TcQ9l1JkQHbe3Y9+FG0Tmzb5nAqIClWWKfYkQKr3HY3DNkUELEitQOt11rUEoTIhVaMplO5MjMcUhyaOkRfE1EwzRJDuTodvwv6GFBJNbxL5/V1V5ccbxwDK4tVtu1prMp44ddJ43+j4rqfoh+/drPnl+o9FUs7RDRZHI0r/xZnsu0SgSozKmL98ZWtg/0L5ZREW5SrIyP+O9aKbXxobcdcnN/hB5R8E327DWIsGrd6hAcGVVW4DtQqmMCthtP56pYPdAco564u0zJtgqoE7elRjXEir+jqaBZLjMjT9t5iKHKbaDKbRIGh0A4yWnse1c3+h8jv8CaFPIGhVzmzQ3vtKWaDkj5x9ahIoYfBc3kAe3ZVxZk0yjnlC+zcExfznsk7xlASjHiyvvd715Y4/D+hX+BgqDo3EVVv7KqxUzgOSjmRrXjhwLldeL/M5ZBFCJSocR6EY8YeGIH8h2VRe00lqQSU2Jlhh//jRyKPUneqaMzsncMCOROqjTYmSnNhYzMSpQ8jKSQQWWlX7Fs4URhDjs9QsVrXS3SIOU4KWIq3iU4DVm4/0CZ4ZNjyO/btV6yN4ZJx9MxZGfYvxWDXvZli/5Z3nVE6ySAsgb5bJDwj4GzT9dP6TB/Se3UmsCBXDaCuEjM5B21N99IsLITJ0Qq3fnvzeNNDmNXtus1WEvVSK+qHRdSlSmoW4wSymRncB7CbbdrfUSkAazVHSUYxs6KZxKlR9qfdcvsy9slDkJkyLxr6omRO3g4wfpsU6S5IzKJJLOkOZVZCCv00YcOHp3czVn1AxpLlFRdqHlly4KwiStRv17goFS/z3qoDP5wi+jT8FNleUhq5Isgpd5DtEOV3V80qMrjdBW0UV8yAkULFB38FwXXsTExvV00Mp5bFX7oHehy0W9jQmJI8hT91/gXq+ZX+l7xOqsu+RKRlQ7LRjv8I+bF7R/W5e5vJIPkR4DpDilxvSD/kSrPDcbtmdfck1Dlnv30ME00+8XxTCmTsaxqRVcQsKaK64NiWNUOVO60Y8ecfwSnNOtyoxA2BzLoWKdqmX/H5sfN9rOMQkuUH4eUIFKlpDyWWSaGnOJy6ekOJcumJ7fxsaCvj8/M3qxqTwGlvP767YNkiclmbziGjUzpqFe67O6Y96c2+2OKzdPM8bXiHo0VvCUSTO9tiZmbQ7KIZfV4G60rwxIZj5w==</t>
+          <t>yVjpCgZpNvOHlEoAN60+iXcNR8qcjD2afR3U+XlDrUTEX5W5KWYQZl2WlS6znR8JdtRv8fy9hcGzGgX1t8jwbDwAx0EUQZsw3ZWNu8RJYhGO4TcQ9l1JkQHbe3Y9+FG0Tmzb5nAqIClWWKfYkQKr3HY3DNkUELEitQOt11rUEoTIhVaMplO5MjMcUhyaOkRfE1EwzRJDuTodvwv6GFBJNbxL5/V1V5ccbxwDK4tVtu1prMp44ddJ43+j4rqfoh+/drPnl+o9FUs7RDRZHI0r/xZnsu0SgSozKmL98ZWtg/0L5ZREW5SrIyP+O9aKbXxobcdcnN/hB5R8E327DWIsGrd6hAcGVVW4DtQqmMCthtP56pYPdAco564u0zJtgqoE7elRjXEir+jqaBZLjMjT9t5iKHKbaDKbRIGh0A4yWnse1c3+h8jv8CaFPIGhVzmzQ3vtKWaDkj5x9ahIoYfBc3kAe3ZVxZk0yjnlC+zcExfznsk7xlASjHiyvvd715Y4/D+hX+BgqDo3EVVv7KqxUzgOSjmRrXjhwLldeL/M5ZBFCJSocR6EY8YeGIH8h2VRe00lqQSU2Jlhh//jRyKPUneqaMzsncMCOROqjTYmSnNhYzMSpQ8jKSQQWWlX7Fs4URhDjs9QsVrXS3SIOU4KWIq3iU4DVm4/0CZ4ZNjyO/btV6yN4ZJx9MxZGfYvxWDXvZli/5Z3nVE6ySAsgb5bJDwj4GzT9dP6TB/Se3UmsCBXDaCuEjM5B21N99IsLITJ0Qq3fnvzeNNDmNXtus1WEvVSK+qHRdSlSmoW4wSymRncB7CbbdrfUSkAazVHSUYxs6KZxKlR9qfdcvsy9slDkJkyLxr6omRO3g4wfpsU6S5IzKJJLOkOZVZCCv00YcOHp3czVn1AxpLlFRdqHlly4KwiStRv17goFS/z3qoDP5wi+jT8FNleUhq5Isgpd5DtEOV3V80qMrjdBW0UV8yAkULFB38FwXXsTExvV00Mp5bFX7oHehy0W9jQmJI8hT91/gXq+ZX+l7xOqsu+RKRlQ7LRjv8I+bF7R/W5e5vJIPkR4DpDilxvSD/kSrPDcbtmdfck1Dlnv30ME00+8XxTCmTsaxqRVcQsKaK64NiWNUOVO60Y8ecfwSnNOtyoxA2BQzBsmbXjZrW6P9nfnnvN9ihWabMsRi8mt9X4YSmPGNlHNsHwu2uV9skdd+7KwWsuBvkOEzN6Udmo12ngu2SiBzEDFZ9e05r58YQTqnV4Tgq2FRoSPUUbZPfK5wxDA3Brl7g1akJ5D5hY5XNRV79now==</t>
         </r>
       </text>
     </comment>
@@ -1320,10 +1320,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C3330"/>
+  <dimension ref="A1:C3331"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A3285" workbookViewId="0">
+      <selection activeCell="C3330" sqref="C3330"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
@@ -37924,13 +37924,24 @@
         <v>3944</v>
       </c>
     </row>
-    <row r="3328" spans="1:1">
-      <c r="A3328" s="6" t="s">
-        <v>9</v>
+    <row r="3328" ht="14" customHeight="1" spans="1:3">
+      <c r="A3328" s="4">
+        <v>45258</v>
+      </c>
+      <c r="B3328" s="5">
+        <v>3893</v>
+      </c>
+      <c r="C3328" s="5">
+        <v>3918</v>
       </c>
     </row>
     <row r="3330" spans="1:1">
       <c r="A3330" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3331" spans="1:1">
+      <c r="A3331" s="6" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add merge_data method to merge data from data index
</commit_message>
<xml_diff>
--- a/steel/data/mid-stream/螺纹钢/螺纹钢期货价格.xlsx
+++ b/steel/data/mid-stream/螺纹钢/螺纹钢期货价格.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="14055"/>
+    <workbookView windowWidth="23040" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
             <rFont val="宋体"/>
             <charset val="134"/>
           </rPr>
-          <t>yVjpCgZpNvOHlEoAN60+iXcNR8qcjD2afR3U+XlDrUTEX5W5KWYQZl2WlS6znR8JdtRv8fy9hcGzGgX1t8jwbDwAx0EUQZsw3ZWNu8RJYhGO4TcQ9l1JkQHbe3Y9+FG0Tmzb5nAqIClWWKfYkQKr3HY3DNkUELEitQOt11rUEoTIhVaMplO5MjMcUhyaOkRfE1EwzRJDuTodvwv6GFBJNbxL5/V1V5ccbxwDK4tVtu1prMp44ddJ43+j4rqfoh+/drPnl+o9FUs7RDRZHI0r/xZnsu0SgSozKmL98ZWtg/0L5ZREW5SrIyP+O9aKbXxobcdcnN/hB5R8E327DWIsGrd6hAcGVVW4DtQqmMCthtP56pYPdAco564u0zJtgqoE7elRjXEir+jqaBZLjMjT9t5iKHKbaDKbRIGh0A4yWnse1c3+h8jv8CaFPIGhVzmzQ3vtKWaDkj5x9ahIoYfBc3kAe3ZVxZk0yjnlC+zcExfznsk7xlASjHiyvvd715Y4/D+hX+BgqDo3EVVv7KqxUzgOSjmRrXjhwLldeL/M5ZBFCJSocR6EY8YeGIH8h2VRe00lqQSU2Jlhh//jRyKPUneqaMzsncMCOROqjTYmSnNhYzMSpQ8jKSQQWWlX7Fs4URhDjs9QsVrXS3SIOU4KWIq3iU4DVm4/0CZ4ZNjyO/btV6yN4ZJx9MxZGfYvxWDXvZli/5Z3nVE6ySAsgb5bJDwj4GzT9dP6TB/Se3UmsCBXDaCuEjM5B21N99IsLITJ0Qq3fnvzeNNDmNXtus1WEvVSK+qHRdSlSmoW4wSymRncB7CbbdrfUSkAazVHSUYxs6KZxKlR9qfdcvsy9slDkJkyLxr6omRO3g4wfpsU6S5IzKJJLOkOZVZCCv00YcOHp3czVn1AxpLlFRdqHlly4KwiStRv17goFS/z3qoDP5wi+jT8FNleUhq5Isgpd5DtEOV3V80qMrjdBW0UV8yAkULFB38FwXXsTExvV00Mp5bFX7oHehy0W9jQmJI8hT91/gXq+ZX+l7xOqsu+RKRlQ7LRjv8I+bF7R/W5e5vJIPkR4DpDilxvSD/kSrPDcbtmdfck1Dlnv30ME00+8XxTCmTsaxqRVcQsKaK64NiWNUOVO60Y8ecfwSnNOtyoxA2BQzBsmbXjZrW6P9nfnnvN9ihWabMsRi8mt9X4YSmPGNlHNsHwu2uV9skdd+7KwWsuBvkOEzN6Udmo12ngu2SiBzEDFZ9e05r58YQTqnV4Tgq2FRoSPUUbZPfK5wxDA3Brl7g1akJ5D5hY5XNRV79now==</t>
+          <t>yVjpCgZpNvOHlEoAN60+iXcNR8qcjD2afR3U+XlDrUTEX5W5KWYQZl2WlS6znR8JdtRv8fy9hcGzGgX1t8jwbDwAx0EUQZsw3ZWNu8RJYhGO4TcQ9l1JkQHbe3Y9+FG0Tmzb5nAqIClWWKfYkQKr3HY3DNkUELEitQOt11rUEoTIhVaMplO5MjMcUhyaOkRfE1EwzRJDuTodvwv6GFBJNbxL5/V1V5ccbxwDK4tVtu1prMp44ddJ43+j4rqfoh+/drPnl+o9FUs7RDRZHI0r/xZnsu0SgSozKmL98ZWtg/0L5ZREW5SrIyP+O9aKbXxobcdcnN/hB5R8E327DWIsGrd6hAcGVVW4DtQqmMCthtP56pYPdAco564u0zJtgqoE7elRjXEir+jqaBZLjMjT9t5iKHKbaDKbRIGh0A4yWnse1c3+h8jv8CaFPIGhVzmzQ3vtKWaDkj5x9ahIoYfBc3kAe3ZVxZk0yjnlC+zcExfznsk7xlASjHiyvvd715Y4/D+hX+BgqDo3EVVv7KqxUzgOSjmRrXjhwLldeL/M5ZBFCJSocR6EY8YeGIH8h2VRe00lqQSU2Jlhh//jRyKPUneqaMzsncMCOROqjTYmSnNhYzMSpQ8jKSQQWWlX7Fs4URhDjs9QsVrXS3SIOU4KWIq3iU4DVm4/0CZ4ZNjyO/btV6yN4ZJx9MxZGfYvxWDXvZli/5Z3nVE6ySAsgb5bJDwj4GzT9dP6TB/Se3UmsCBXDaCuEjM5B21N99IsLITJ0Qq3fnvzeNNDmNXtus1WEvVSK+qHRdSlSmoW4wSymRncB7CbbdrfUSkAazVHSUYxs6KZxKlR9qfdcvsy9slDkJkyLxr6omRO3g4wfpsU6S5IzKJJLOkOZVZCCv00YcOHp3czVn1AxpLlFRdqHlly4KwiStRv17goFS/z3qoDP5wi+jT8FNleUhq5Isgpd5DtEOV3V80qMrjdBW0UV8yAkULFB38FwXXsTExvV00Mp5bFX7oHehy0W9jQmJI8hT91/gXq+ZX+l7xOqsu+RKRlQ7LRjv8I+bF7R/W5e5vJIPkR4DpDilxvSD/kSrPDcbtmdfck1Dlnv30ME00+8XxTCmTsaxqRVcQsKaK64NiWNUOVO60Y8ecfwSnNOtyoxA2BzLoWKdqmX/GFKO72112kKHHB9Q7Gw9ScmTnTxwVtWMzqTvhRW521E8vjqyfbfcWE9CxAxjsjaJ5T9P37wdCte3WhGEvqDIK/igZ7NvN7wvQOS/yT3i/ITRA5v5ZZ8yvGB7oCFJGkaAE8kLo9vIDZww==</t>
         </r>
       </text>
     </comment>
@@ -1320,16 +1320,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C3331"/>
+  <dimension ref="A1:C3333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3285" workbookViewId="0">
-      <selection activeCell="C3330" sqref="C3330"/>
+    <sheetView tabSelected="1" topLeftCell="A3309" workbookViewId="0">
+      <selection activeCell="C3334" sqref="C3334"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="8.875" customWidth="1"/>
-    <col min="2" max="3" width="20.125" customWidth="1"/>
+    <col min="1" max="1" width="10.4444444444444" customWidth="1"/>
+    <col min="2" max="3" width="22.2222222222222" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="20" customHeight="1" spans="1:1">
@@ -37935,13 +37935,35 @@
         <v>3918</v>
       </c>
     </row>
-    <row r="3330" spans="1:1">
-      <c r="A3330" s="6" t="s">
-        <v>9</v>
+    <row r="3329" ht="14" customHeight="1" spans="1:3">
+      <c r="A3329" s="4">
+        <v>45259</v>
+      </c>
+      <c r="B3329" s="5">
+        <v>3896</v>
+      </c>
+      <c r="C3329" s="5">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="3330" ht="14" customHeight="1" spans="1:3">
+      <c r="A3330" s="4">
+        <v>45260</v>
+      </c>
+      <c r="B3330" s="5">
+        <v>3934</v>
+      </c>
+      <c r="C3330" s="5">
+        <v>3911</v>
       </c>
     </row>
     <row r="3331" spans="1:1">
       <c r="A3331" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3333" spans="1:1">
+      <c r="A3333" s="6" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>